<commit_message>
Calibrating SoCEUtiNTY and SoCDTtiNTY, updates to BPEic and PERAC based on new categorization
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A11046-15F1-4BB2-86A2-BDBE51E36B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="7800" yWindow="1995" windowWidth="9465" windowHeight="8250" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,18 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1176,7 +1188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1411,23 +1423,23 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,6 +1530,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1553,6 +1582,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1728,10 +1774,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1923,7 +1969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1996,7 +2042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14158,46 +14204,46 @@
     </row>
     <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="35" t="s">
+      <c r="B142" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="35"/>
-      <c r="D142" s="35"/>
-      <c r="E142" s="35"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="35"/>
-      <c r="H142" s="35"/>
-      <c r="I142" s="35"/>
-      <c r="J142" s="35"/>
-      <c r="K142" s="35"/>
-      <c r="L142" s="35"/>
-      <c r="M142" s="35"/>
-      <c r="N142" s="35"/>
-      <c r="O142" s="35"/>
-      <c r="P142" s="35"/>
-      <c r="Q142" s="35"/>
-      <c r="R142" s="35"/>
-      <c r="S142" s="35"/>
-      <c r="T142" s="35"/>
-      <c r="U142" s="35"/>
-      <c r="V142" s="35"/>
-      <c r="W142" s="35"/>
-      <c r="X142" s="35"/>
-      <c r="Y142" s="35"/>
-      <c r="Z142" s="35"/>
-      <c r="AA142" s="35"/>
-      <c r="AB142" s="35"/>
-      <c r="AC142" s="35"/>
-      <c r="AD142" s="35"/>
-      <c r="AE142" s="35"/>
-      <c r="AF142" s="35"/>
-      <c r="AG142" s="35"/>
-      <c r="AH142" s="35"/>
-      <c r="AI142" s="35"/>
-      <c r="AJ142" s="35"/>
-      <c r="AK142" s="35"/>
-      <c r="AL142" s="35"/>
-      <c r="AM142" s="35"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="36"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+      <c r="I142" s="36"/>
+      <c r="J142" s="36"/>
+      <c r="K142" s="36"/>
+      <c r="L142" s="36"/>
+      <c r="M142" s="36"/>
+      <c r="N142" s="36"/>
+      <c r="O142" s="36"/>
+      <c r="P142" s="36"/>
+      <c r="Q142" s="36"/>
+      <c r="R142" s="36"/>
+      <c r="S142" s="36"/>
+      <c r="T142" s="36"/>
+      <c r="U142" s="36"/>
+      <c r="V142" s="36"/>
+      <c r="W142" s="36"/>
+      <c r="X142" s="36"/>
+      <c r="Y142" s="36"/>
+      <c r="Z142" s="36"/>
+      <c r="AA142" s="36"/>
+      <c r="AB142" s="36"/>
+      <c r="AC142" s="36"/>
+      <c r="AD142" s="36"/>
+      <c r="AE142" s="36"/>
+      <c r="AF142" s="36"/>
+      <c r="AG142" s="36"/>
+      <c r="AH142" s="36"/>
+      <c r="AI142" s="36"/>
+      <c r="AJ142" s="36"/>
+      <c r="AK142" s="36"/>
+      <c r="AL142" s="36"/>
+      <c r="AM142" s="36"/>
     </row>
     <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
@@ -14309,7 +14355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23843,46 +23889,46 @@
     </row>
     <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="35"/>
-      <c r="H118" s="35"/>
-      <c r="I118" s="35"/>
-      <c r="J118" s="35"/>
-      <c r="K118" s="35"/>
-      <c r="L118" s="35"/>
-      <c r="M118" s="35"/>
-      <c r="N118" s="35"/>
-      <c r="O118" s="35"/>
-      <c r="P118" s="35"/>
-      <c r="Q118" s="35"/>
-      <c r="R118" s="35"/>
-      <c r="S118" s="35"/>
-      <c r="T118" s="35"/>
-      <c r="U118" s="35"/>
-      <c r="V118" s="35"/>
-      <c r="W118" s="35"/>
-      <c r="X118" s="35"/>
-      <c r="Y118" s="35"/>
-      <c r="Z118" s="35"/>
-      <c r="AA118" s="35"/>
-      <c r="AB118" s="35"/>
-      <c r="AC118" s="35"/>
-      <c r="AD118" s="35"/>
-      <c r="AE118" s="35"/>
-      <c r="AF118" s="35"/>
-      <c r="AG118" s="35"/>
-      <c r="AH118" s="35"/>
-      <c r="AI118" s="35"/>
-      <c r="AJ118" s="35"/>
-      <c r="AK118" s="35"/>
-      <c r="AL118" s="35"/>
-      <c r="AM118" s="35"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="36"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="36"/>
+      <c r="I118" s="36"/>
+      <c r="J118" s="36"/>
+      <c r="K118" s="36"/>
+      <c r="L118" s="36"/>
+      <c r="M118" s="36"/>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="36"/>
+      <c r="Q118" s="36"/>
+      <c r="R118" s="36"/>
+      <c r="S118" s="36"/>
+      <c r="T118" s="36"/>
+      <c r="U118" s="36"/>
+      <c r="V118" s="36"/>
+      <c r="W118" s="36"/>
+      <c r="X118" s="36"/>
+      <c r="Y118" s="36"/>
+      <c r="Z118" s="36"/>
+      <c r="AA118" s="36"/>
+      <c r="AB118" s="36"/>
+      <c r="AC118" s="36"/>
+      <c r="AD118" s="36"/>
+      <c r="AE118" s="36"/>
+      <c r="AF118" s="36"/>
+      <c r="AG118" s="36"/>
+      <c r="AH118" s="36"/>
+      <c r="AI118" s="36"/>
+      <c r="AJ118" s="36"/>
+      <c r="AK118" s="36"/>
+      <c r="AL118" s="36"/>
+      <c r="AM118" s="36"/>
     </row>
     <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
@@ -23999,7 +24045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26209,7 +26255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26341,13 +26387,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26358,7 +26406,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26376,14 +26424,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.5699999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>4.5699999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>4.7800000000000002E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Jun's Oct 9th updates to MN data
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A11046-15F1-4BB2-86A2-BDBE51E36B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="1995" windowWidth="9465" windowHeight="8250" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,18 +20,7 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1188,7 +1176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1423,23 +1411,23 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
+    <cellStyle name="Footnotes: top row" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Parent row" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Table title" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1530,23 +1518,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1582,23 +1553,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1774,10 +1728,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1969,7 +1923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2042,7 +1996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14204,46 +14158,46 @@
     </row>
     <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="36" t="s">
+      <c r="B142" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="36"/>
-      <c r="D142" s="36"/>
-      <c r="E142" s="36"/>
-      <c r="F142" s="36"/>
-      <c r="G142" s="36"/>
-      <c r="H142" s="36"/>
-      <c r="I142" s="36"/>
-      <c r="J142" s="36"/>
-      <c r="K142" s="36"/>
-      <c r="L142" s="36"/>
-      <c r="M142" s="36"/>
-      <c r="N142" s="36"/>
-      <c r="O142" s="36"/>
-      <c r="P142" s="36"/>
-      <c r="Q142" s="36"/>
-      <c r="R142" s="36"/>
-      <c r="S142" s="36"/>
-      <c r="T142" s="36"/>
-      <c r="U142" s="36"/>
-      <c r="V142" s="36"/>
-      <c r="W142" s="36"/>
-      <c r="X142" s="36"/>
-      <c r="Y142" s="36"/>
-      <c r="Z142" s="36"/>
-      <c r="AA142" s="36"/>
-      <c r="AB142" s="36"/>
-      <c r="AC142" s="36"/>
-      <c r="AD142" s="36"/>
-      <c r="AE142" s="36"/>
-      <c r="AF142" s="36"/>
-      <c r="AG142" s="36"/>
-      <c r="AH142" s="36"/>
-      <c r="AI142" s="36"/>
-      <c r="AJ142" s="36"/>
-      <c r="AK142" s="36"/>
-      <c r="AL142" s="36"/>
-      <c r="AM142" s="36"/>
+      <c r="C142" s="35"/>
+      <c r="D142" s="35"/>
+      <c r="E142" s="35"/>
+      <c r="F142" s="35"/>
+      <c r="G142" s="35"/>
+      <c r="H142" s="35"/>
+      <c r="I142" s="35"/>
+      <c r="J142" s="35"/>
+      <c r="K142" s="35"/>
+      <c r="L142" s="35"/>
+      <c r="M142" s="35"/>
+      <c r="N142" s="35"/>
+      <c r="O142" s="35"/>
+      <c r="P142" s="35"/>
+      <c r="Q142" s="35"/>
+      <c r="R142" s="35"/>
+      <c r="S142" s="35"/>
+      <c r="T142" s="35"/>
+      <c r="U142" s="35"/>
+      <c r="V142" s="35"/>
+      <c r="W142" s="35"/>
+      <c r="X142" s="35"/>
+      <c r="Y142" s="35"/>
+      <c r="Z142" s="35"/>
+      <c r="AA142" s="35"/>
+      <c r="AB142" s="35"/>
+      <c r="AC142" s="35"/>
+      <c r="AD142" s="35"/>
+      <c r="AE142" s="35"/>
+      <c r="AF142" s="35"/>
+      <c r="AG142" s="35"/>
+      <c r="AH142" s="35"/>
+      <c r="AI142" s="35"/>
+      <c r="AJ142" s="35"/>
+      <c r="AK142" s="35"/>
+      <c r="AL142" s="35"/>
+      <c r="AM142" s="35"/>
     </row>
     <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
@@ -14355,7 +14309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23889,46 +23843,46 @@
     </row>
     <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="36" t="s">
+      <c r="B118" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="36"/>
-      <c r="K118" s="36"/>
-      <c r="L118" s="36"/>
-      <c r="M118" s="36"/>
-      <c r="N118" s="36"/>
-      <c r="O118" s="36"/>
-      <c r="P118" s="36"/>
-      <c r="Q118" s="36"/>
-      <c r="R118" s="36"/>
-      <c r="S118" s="36"/>
-      <c r="T118" s="36"/>
-      <c r="U118" s="36"/>
-      <c r="V118" s="36"/>
-      <c r="W118" s="36"/>
-      <c r="X118" s="36"/>
-      <c r="Y118" s="36"/>
-      <c r="Z118" s="36"/>
-      <c r="AA118" s="36"/>
-      <c r="AB118" s="36"/>
-      <c r="AC118" s="36"/>
-      <c r="AD118" s="36"/>
-      <c r="AE118" s="36"/>
-      <c r="AF118" s="36"/>
-      <c r="AG118" s="36"/>
-      <c r="AH118" s="36"/>
-      <c r="AI118" s="36"/>
-      <c r="AJ118" s="36"/>
-      <c r="AK118" s="36"/>
-      <c r="AL118" s="36"/>
-      <c r="AM118" s="36"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="35"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="35"/>
+      <c r="H118" s="35"/>
+      <c r="I118" s="35"/>
+      <c r="J118" s="35"/>
+      <c r="K118" s="35"/>
+      <c r="L118" s="35"/>
+      <c r="M118" s="35"/>
+      <c r="N118" s="35"/>
+      <c r="O118" s="35"/>
+      <c r="P118" s="35"/>
+      <c r="Q118" s="35"/>
+      <c r="R118" s="35"/>
+      <c r="S118" s="35"/>
+      <c r="T118" s="35"/>
+      <c r="U118" s="35"/>
+      <c r="V118" s="35"/>
+      <c r="W118" s="35"/>
+      <c r="X118" s="35"/>
+      <c r="Y118" s="35"/>
+      <c r="Z118" s="35"/>
+      <c r="AA118" s="35"/>
+      <c r="AB118" s="35"/>
+      <c r="AC118" s="35"/>
+      <c r="AD118" s="35"/>
+      <c r="AE118" s="35"/>
+      <c r="AF118" s="35"/>
+      <c r="AG118" s="35"/>
+      <c r="AH118" s="35"/>
+      <c r="AI118" s="35"/>
+      <c r="AJ118" s="35"/>
+      <c r="AK118" s="35"/>
+      <c r="AL118" s="35"/>
+      <c r="AM118" s="35"/>
     </row>
     <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
@@ -24045,7 +23999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26255,7 +26209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26387,15 +26341,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26406,7 +26358,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26424,14 +26376,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.8000000000000001E-2</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C2" s="4">
         <f>B2</f>
-        <v>4.8000000000000001E-2</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>0.05</v>
+        <v>4.7800000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibration files and Reference scenario
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BC7D3-4F4A-41D8-B33A-00B02C371BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="11610" yWindow="2910" windowWidth="16185" windowHeight="12945" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,18 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1176,7 +1188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1411,23 +1423,23 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,6 +1530,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1553,6 +1582,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1728,10 +1774,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1923,7 +1969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1996,7 +2042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14158,46 +14204,46 @@
     </row>
     <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="35" t="s">
+      <c r="B142" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="35"/>
-      <c r="D142" s="35"/>
-      <c r="E142" s="35"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="35"/>
-      <c r="H142" s="35"/>
-      <c r="I142" s="35"/>
-      <c r="J142" s="35"/>
-      <c r="K142" s="35"/>
-      <c r="L142" s="35"/>
-      <c r="M142" s="35"/>
-      <c r="N142" s="35"/>
-      <c r="O142" s="35"/>
-      <c r="P142" s="35"/>
-      <c r="Q142" s="35"/>
-      <c r="R142" s="35"/>
-      <c r="S142" s="35"/>
-      <c r="T142" s="35"/>
-      <c r="U142" s="35"/>
-      <c r="V142" s="35"/>
-      <c r="W142" s="35"/>
-      <c r="X142" s="35"/>
-      <c r="Y142" s="35"/>
-      <c r="Z142" s="35"/>
-      <c r="AA142" s="35"/>
-      <c r="AB142" s="35"/>
-      <c r="AC142" s="35"/>
-      <c r="AD142" s="35"/>
-      <c r="AE142" s="35"/>
-      <c r="AF142" s="35"/>
-      <c r="AG142" s="35"/>
-      <c r="AH142" s="35"/>
-      <c r="AI142" s="35"/>
-      <c r="AJ142" s="35"/>
-      <c r="AK142" s="35"/>
-      <c r="AL142" s="35"/>
-      <c r="AM142" s="35"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="36"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+      <c r="I142" s="36"/>
+      <c r="J142" s="36"/>
+      <c r="K142" s="36"/>
+      <c r="L142" s="36"/>
+      <c r="M142" s="36"/>
+      <c r="N142" s="36"/>
+      <c r="O142" s="36"/>
+      <c r="P142" s="36"/>
+      <c r="Q142" s="36"/>
+      <c r="R142" s="36"/>
+      <c r="S142" s="36"/>
+      <c r="T142" s="36"/>
+      <c r="U142" s="36"/>
+      <c r="V142" s="36"/>
+      <c r="W142" s="36"/>
+      <c r="X142" s="36"/>
+      <c r="Y142" s="36"/>
+      <c r="Z142" s="36"/>
+      <c r="AA142" s="36"/>
+      <c r="AB142" s="36"/>
+      <c r="AC142" s="36"/>
+      <c r="AD142" s="36"/>
+      <c r="AE142" s="36"/>
+      <c r="AF142" s="36"/>
+      <c r="AG142" s="36"/>
+      <c r="AH142" s="36"/>
+      <c r="AI142" s="36"/>
+      <c r="AJ142" s="36"/>
+      <c r="AK142" s="36"/>
+      <c r="AL142" s="36"/>
+      <c r="AM142" s="36"/>
     </row>
     <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
@@ -14309,7 +14355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23843,46 +23889,46 @@
     </row>
     <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="35"/>
-      <c r="H118" s="35"/>
-      <c r="I118" s="35"/>
-      <c r="J118" s="35"/>
-      <c r="K118" s="35"/>
-      <c r="L118" s="35"/>
-      <c r="M118" s="35"/>
-      <c r="N118" s="35"/>
-      <c r="O118" s="35"/>
-      <c r="P118" s="35"/>
-      <c r="Q118" s="35"/>
-      <c r="R118" s="35"/>
-      <c r="S118" s="35"/>
-      <c r="T118" s="35"/>
-      <c r="U118" s="35"/>
-      <c r="V118" s="35"/>
-      <c r="W118" s="35"/>
-      <c r="X118" s="35"/>
-      <c r="Y118" s="35"/>
-      <c r="Z118" s="35"/>
-      <c r="AA118" s="35"/>
-      <c r="AB118" s="35"/>
-      <c r="AC118" s="35"/>
-      <c r="AD118" s="35"/>
-      <c r="AE118" s="35"/>
-      <c r="AF118" s="35"/>
-      <c r="AG118" s="35"/>
-      <c r="AH118" s="35"/>
-      <c r="AI118" s="35"/>
-      <c r="AJ118" s="35"/>
-      <c r="AK118" s="35"/>
-      <c r="AL118" s="35"/>
-      <c r="AM118" s="35"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="36"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="36"/>
+      <c r="I118" s="36"/>
+      <c r="J118" s="36"/>
+      <c r="K118" s="36"/>
+      <c r="L118" s="36"/>
+      <c r="M118" s="36"/>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="36"/>
+      <c r="Q118" s="36"/>
+      <c r="R118" s="36"/>
+      <c r="S118" s="36"/>
+      <c r="T118" s="36"/>
+      <c r="U118" s="36"/>
+      <c r="V118" s="36"/>
+      <c r="W118" s="36"/>
+      <c r="X118" s="36"/>
+      <c r="Y118" s="36"/>
+      <c r="Z118" s="36"/>
+      <c r="AA118" s="36"/>
+      <c r="AB118" s="36"/>
+      <c r="AC118" s="36"/>
+      <c r="AD118" s="36"/>
+      <c r="AE118" s="36"/>
+      <c r="AF118" s="36"/>
+      <c r="AG118" s="36"/>
+      <c r="AH118" s="36"/>
+      <c r="AI118" s="36"/>
+      <c r="AJ118" s="36"/>
+      <c r="AK118" s="36"/>
+      <c r="AL118" s="36"/>
+      <c r="AM118" s="36"/>
     </row>
     <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
@@ -23999,7 +24045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26209,7 +26255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26341,13 +26387,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26358,7 +26406,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26376,14 +26424,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.5699999999999998E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C2" s="4">
-        <f>B2</f>
-        <v>4.5699999999999998E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>4.7800000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26391,14 +26438,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>5.7000000000000002E-2</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="C3" s="4">
-        <f>B3</f>
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D3" s="34">
-        <v>6.2E-2</v>
+        <v>6.1499999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26420,14 +26466,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="34">
-        <v>0.114</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="C5" s="4">
-        <f>B5</f>
-        <v>0.114</v>
+        <v>0.47</v>
       </c>
       <c r="D5" s="34">
-        <v>0.112</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26435,14 +26480,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>7.1499999999999994E-2</v>
+        <v>0.125</v>
       </c>
       <c r="C6" s="4">
-        <f>B6</f>
-        <v>7.1499999999999994E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D6" s="34">
-        <v>7.1199999999999999E-2</v>
+        <v>0.22900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26453,7 +26497,6 @@
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="C7" s="4">
-        <f>B7</f>
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="D7" s="34">

</xml_diff>

<commit_message>
MN Specific files: BPEIC, PERAC, BLAPE, calibration for bldg, transp
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BC7D3-4F4A-41D8-B33A-00B02C371BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="11610" yWindow="2910" windowWidth="16185" windowHeight="12945" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,18 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1176,7 +1188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1411,23 +1423,23 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1518,6 +1530,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1553,6 +1582,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1728,10 +1774,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1923,7 +1969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1996,7 +2042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14158,46 +14204,46 @@
     </row>
     <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="35" t="s">
+      <c r="B142" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="35"/>
-      <c r="D142" s="35"/>
-      <c r="E142" s="35"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="35"/>
-      <c r="H142" s="35"/>
-      <c r="I142" s="35"/>
-      <c r="J142" s="35"/>
-      <c r="K142" s="35"/>
-      <c r="L142" s="35"/>
-      <c r="M142" s="35"/>
-      <c r="N142" s="35"/>
-      <c r="O142" s="35"/>
-      <c r="P142" s="35"/>
-      <c r="Q142" s="35"/>
-      <c r="R142" s="35"/>
-      <c r="S142" s="35"/>
-      <c r="T142" s="35"/>
-      <c r="U142" s="35"/>
-      <c r="V142" s="35"/>
-      <c r="W142" s="35"/>
-      <c r="X142" s="35"/>
-      <c r="Y142" s="35"/>
-      <c r="Z142" s="35"/>
-      <c r="AA142" s="35"/>
-      <c r="AB142" s="35"/>
-      <c r="AC142" s="35"/>
-      <c r="AD142" s="35"/>
-      <c r="AE142" s="35"/>
-      <c r="AF142" s="35"/>
-      <c r="AG142" s="35"/>
-      <c r="AH142" s="35"/>
-      <c r="AI142" s="35"/>
-      <c r="AJ142" s="35"/>
-      <c r="AK142" s="35"/>
-      <c r="AL142" s="35"/>
-      <c r="AM142" s="35"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+      <c r="E142" s="36"/>
+      <c r="F142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="36"/>
+      <c r="I142" s="36"/>
+      <c r="J142" s="36"/>
+      <c r="K142" s="36"/>
+      <c r="L142" s="36"/>
+      <c r="M142" s="36"/>
+      <c r="N142" s="36"/>
+      <c r="O142" s="36"/>
+      <c r="P142" s="36"/>
+      <c r="Q142" s="36"/>
+      <c r="R142" s="36"/>
+      <c r="S142" s="36"/>
+      <c r="T142" s="36"/>
+      <c r="U142" s="36"/>
+      <c r="V142" s="36"/>
+      <c r="W142" s="36"/>
+      <c r="X142" s="36"/>
+      <c r="Y142" s="36"/>
+      <c r="Z142" s="36"/>
+      <c r="AA142" s="36"/>
+      <c r="AB142" s="36"/>
+      <c r="AC142" s="36"/>
+      <c r="AD142" s="36"/>
+      <c r="AE142" s="36"/>
+      <c r="AF142" s="36"/>
+      <c r="AG142" s="36"/>
+      <c r="AH142" s="36"/>
+      <c r="AI142" s="36"/>
+      <c r="AJ142" s="36"/>
+      <c r="AK142" s="36"/>
+      <c r="AL142" s="36"/>
+      <c r="AM142" s="36"/>
     </row>
     <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
@@ -14309,7 +14355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23843,46 +23889,46 @@
     </row>
     <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="35"/>
-      <c r="H118" s="35"/>
-      <c r="I118" s="35"/>
-      <c r="J118" s="35"/>
-      <c r="K118" s="35"/>
-      <c r="L118" s="35"/>
-      <c r="M118" s="35"/>
-      <c r="N118" s="35"/>
-      <c r="O118" s="35"/>
-      <c r="P118" s="35"/>
-      <c r="Q118" s="35"/>
-      <c r="R118" s="35"/>
-      <c r="S118" s="35"/>
-      <c r="T118" s="35"/>
-      <c r="U118" s="35"/>
-      <c r="V118" s="35"/>
-      <c r="W118" s="35"/>
-      <c r="X118" s="35"/>
-      <c r="Y118" s="35"/>
-      <c r="Z118" s="35"/>
-      <c r="AA118" s="35"/>
-      <c r="AB118" s="35"/>
-      <c r="AC118" s="35"/>
-      <c r="AD118" s="35"/>
-      <c r="AE118" s="35"/>
-      <c r="AF118" s="35"/>
-      <c r="AG118" s="35"/>
-      <c r="AH118" s="35"/>
-      <c r="AI118" s="35"/>
-      <c r="AJ118" s="35"/>
-      <c r="AK118" s="35"/>
-      <c r="AL118" s="35"/>
-      <c r="AM118" s="35"/>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="36"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="36"/>
+      <c r="I118" s="36"/>
+      <c r="J118" s="36"/>
+      <c r="K118" s="36"/>
+      <c r="L118" s="36"/>
+      <c r="M118" s="36"/>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="36"/>
+      <c r="Q118" s="36"/>
+      <c r="R118" s="36"/>
+      <c r="S118" s="36"/>
+      <c r="T118" s="36"/>
+      <c r="U118" s="36"/>
+      <c r="V118" s="36"/>
+      <c r="W118" s="36"/>
+      <c r="X118" s="36"/>
+      <c r="Y118" s="36"/>
+      <c r="Z118" s="36"/>
+      <c r="AA118" s="36"/>
+      <c r="AB118" s="36"/>
+      <c r="AC118" s="36"/>
+      <c r="AD118" s="36"/>
+      <c r="AE118" s="36"/>
+      <c r="AF118" s="36"/>
+      <c r="AG118" s="36"/>
+      <c r="AH118" s="36"/>
+      <c r="AI118" s="36"/>
+      <c r="AJ118" s="36"/>
+      <c r="AK118" s="36"/>
+      <c r="AL118" s="36"/>
+      <c r="AM118" s="36"/>
     </row>
     <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
@@ -23999,7 +24045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26209,7 +26255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26341,13 +26387,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26358,7 +26406,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26376,14 +26424,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>4.5699999999999998E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C2" s="4">
-        <f>B2</f>
-        <v>4.5699999999999998E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>4.7800000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26391,14 +26438,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>5.7000000000000002E-2</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="C3" s="4">
-        <f>B3</f>
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D3" s="34">
-        <v>6.2E-2</v>
+        <v>6.1499999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26420,14 +26466,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="34">
-        <v>0.114</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="C5" s="4">
-        <f>B5</f>
-        <v>0.114</v>
+        <v>0.47</v>
       </c>
       <c r="D5" s="34">
-        <v>0.112</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26435,14 +26480,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>7.1499999999999994E-2</v>
+        <v>0.125</v>
       </c>
       <c r="C6" s="4">
-        <f>B6</f>
-        <v>7.1499999999999994E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D6" s="34">
-        <v>7.1199999999999999E-2</v>
+        <v>0.22900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26453,7 +26497,6 @@
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="C7" s="4">
-        <f>B7</f>
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="D7" s="34">

</xml_diff>

<commit_message>
Updated model version and updated calibration
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Minnesota\MN_mod\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BC7D3-4F4A-41D8-B33A-00B02C371BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F2F58D-BA3B-4D89-93A2-6F18CA18D88A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="2910" windowWidth="16185" windowHeight="12945" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15825" yWindow="765" windowWidth="10140" windowHeight="14940" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26394,7 +26394,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26405,7 +26405,7 @@
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>381</v>
       </c>
@@ -26424,13 +26424,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="C2" s="4">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26438,13 +26438,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>6.1800000000000001E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C3" s="4">
-        <v>5.8000000000000003E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D3" s="34">
-        <v>6.1499999999999999E-2</v>
+        <v>6.1899999999999997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26466,13 +26466,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="34">
-        <v>0.48099999999999998</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="C5" s="4">
-        <v>0.47</v>
+        <v>0.11905</v>
       </c>
       <c r="D5" s="34">
-        <v>0.26</v>
+        <v>0.1105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26480,13 +26480,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>0.125</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="C6" s="4">
-        <v>0.125</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="D6" s="34">
-        <v>0.22900000000000001</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26494,13 +26494,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="34">
-        <v>6.7500000000000004E-2</v>
+        <v>6.7280000000000006E-2</v>
       </c>
       <c r="C7" s="4">
-        <v>6.7500000000000004E-2</v>
+        <v>6.7280000000000006E-2</v>
       </c>
       <c r="D7" s="34">
-        <v>6.9500000000000006E-2</v>
+        <v>6.7280000000000006E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RMI updates through 12/2
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BC7D3-4F4A-41D8-B33A-00B02C371BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="2910" windowWidth="16185" windowHeight="12945" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19425" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,18 +20,7 @@
     <sheet name="Pre-Calibration Calculated Vals" sheetId="7" r:id="rId6"/>
     <sheet name="SoCEUtiNTY" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1188,7 +1176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1423,23 +1411,23 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
+    <cellStyle name="Footnotes: top row" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Parent row" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Table title" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1530,23 +1518,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1582,23 +1553,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1774,10 +1728,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1969,7 +1923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2042,7 +1996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14204,46 +14158,46 @@
     </row>
     <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="36" t="s">
+      <c r="B142" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="C142" s="36"/>
-      <c r="D142" s="36"/>
-      <c r="E142" s="36"/>
-      <c r="F142" s="36"/>
-      <c r="G142" s="36"/>
-      <c r="H142" s="36"/>
-      <c r="I142" s="36"/>
-      <c r="J142" s="36"/>
-      <c r="K142" s="36"/>
-      <c r="L142" s="36"/>
-      <c r="M142" s="36"/>
-      <c r="N142" s="36"/>
-      <c r="O142" s="36"/>
-      <c r="P142" s="36"/>
-      <c r="Q142" s="36"/>
-      <c r="R142" s="36"/>
-      <c r="S142" s="36"/>
-      <c r="T142" s="36"/>
-      <c r="U142" s="36"/>
-      <c r="V142" s="36"/>
-      <c r="W142" s="36"/>
-      <c r="X142" s="36"/>
-      <c r="Y142" s="36"/>
-      <c r="Z142" s="36"/>
-      <c r="AA142" s="36"/>
-      <c r="AB142" s="36"/>
-      <c r="AC142" s="36"/>
-      <c r="AD142" s="36"/>
-      <c r="AE142" s="36"/>
-      <c r="AF142" s="36"/>
-      <c r="AG142" s="36"/>
-      <c r="AH142" s="36"/>
-      <c r="AI142" s="36"/>
-      <c r="AJ142" s="36"/>
-      <c r="AK142" s="36"/>
-      <c r="AL142" s="36"/>
-      <c r="AM142" s="36"/>
+      <c r="C142" s="35"/>
+      <c r="D142" s="35"/>
+      <c r="E142" s="35"/>
+      <c r="F142" s="35"/>
+      <c r="G142" s="35"/>
+      <c r="H142" s="35"/>
+      <c r="I142" s="35"/>
+      <c r="J142" s="35"/>
+      <c r="K142" s="35"/>
+      <c r="L142" s="35"/>
+      <c r="M142" s="35"/>
+      <c r="N142" s="35"/>
+      <c r="O142" s="35"/>
+      <c r="P142" s="35"/>
+      <c r="Q142" s="35"/>
+      <c r="R142" s="35"/>
+      <c r="S142" s="35"/>
+      <c r="T142" s="35"/>
+      <c r="U142" s="35"/>
+      <c r="V142" s="35"/>
+      <c r="W142" s="35"/>
+      <c r="X142" s="35"/>
+      <c r="Y142" s="35"/>
+      <c r="Z142" s="35"/>
+      <c r="AA142" s="35"/>
+      <c r="AB142" s="35"/>
+      <c r="AC142" s="35"/>
+      <c r="AD142" s="35"/>
+      <c r="AE142" s="35"/>
+      <c r="AF142" s="35"/>
+      <c r="AG142" s="35"/>
+      <c r="AH142" s="35"/>
+      <c r="AI142" s="35"/>
+      <c r="AJ142" s="35"/>
+      <c r="AK142" s="35"/>
+      <c r="AL142" s="35"/>
+      <c r="AM142" s="35"/>
     </row>
     <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
@@ -14355,7 +14309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23889,46 +23843,46 @@
     </row>
     <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="36" t="s">
+      <c r="B118" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="36"/>
-      <c r="K118" s="36"/>
-      <c r="L118" s="36"/>
-      <c r="M118" s="36"/>
-      <c r="N118" s="36"/>
-      <c r="O118" s="36"/>
-      <c r="P118" s="36"/>
-      <c r="Q118" s="36"/>
-      <c r="R118" s="36"/>
-      <c r="S118" s="36"/>
-      <c r="T118" s="36"/>
-      <c r="U118" s="36"/>
-      <c r="V118" s="36"/>
-      <c r="W118" s="36"/>
-      <c r="X118" s="36"/>
-      <c r="Y118" s="36"/>
-      <c r="Z118" s="36"/>
-      <c r="AA118" s="36"/>
-      <c r="AB118" s="36"/>
-      <c r="AC118" s="36"/>
-      <c r="AD118" s="36"/>
-      <c r="AE118" s="36"/>
-      <c r="AF118" s="36"/>
-      <c r="AG118" s="36"/>
-      <c r="AH118" s="36"/>
-      <c r="AI118" s="36"/>
-      <c r="AJ118" s="36"/>
-      <c r="AK118" s="36"/>
-      <c r="AL118" s="36"/>
-      <c r="AM118" s="36"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="35"/>
+      <c r="F118" s="35"/>
+      <c r="G118" s="35"/>
+      <c r="H118" s="35"/>
+      <c r="I118" s="35"/>
+      <c r="J118" s="35"/>
+      <c r="K118" s="35"/>
+      <c r="L118" s="35"/>
+      <c r="M118" s="35"/>
+      <c r="N118" s="35"/>
+      <c r="O118" s="35"/>
+      <c r="P118" s="35"/>
+      <c r="Q118" s="35"/>
+      <c r="R118" s="35"/>
+      <c r="S118" s="35"/>
+      <c r="T118" s="35"/>
+      <c r="U118" s="35"/>
+      <c r="V118" s="35"/>
+      <c r="W118" s="35"/>
+      <c r="X118" s="35"/>
+      <c r="Y118" s="35"/>
+      <c r="Z118" s="35"/>
+      <c r="AA118" s="35"/>
+      <c r="AB118" s="35"/>
+      <c r="AC118" s="35"/>
+      <c r="AD118" s="35"/>
+      <c r="AE118" s="35"/>
+      <c r="AF118" s="35"/>
+      <c r="AG118" s="35"/>
+      <c r="AH118" s="35"/>
+      <c r="AI118" s="35"/>
+      <c r="AJ118" s="35"/>
+      <c r="AK118" s="35"/>
+      <c r="AL118" s="35"/>
+      <c r="AM118" s="35"/>
     </row>
     <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
@@ -24045,7 +23999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26255,7 +26209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26387,15 +26341,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26406,7 +26358,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>381</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -26424,13 +26376,14 @@
         <v>3</v>
       </c>
       <c r="B2" s="34">
-        <v>5.1999999999999998E-2</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C2" s="4">
-        <v>5.1999999999999998E-2</v>
+        <f>B2</f>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="D2" s="34">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7800000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26438,13 +26391,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="34">
-        <v>6.1800000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="C3" s="4">
-        <v>5.8000000000000003E-2</v>
+        <f>B3</f>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D3" s="34">
-        <v>6.1499999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26466,13 +26420,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="34">
-        <v>0.48099999999999998</v>
+        <v>0.114</v>
       </c>
       <c r="C5" s="4">
-        <v>0.47</v>
+        <f>B5</f>
+        <v>0.114</v>
       </c>
       <c r="D5" s="34">
-        <v>0.26</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26480,13 +26435,14 @@
         <v>7</v>
       </c>
       <c r="B6" s="34">
-        <v>0.125</v>
+        <v>7.1499999999999994E-2</v>
       </c>
       <c r="C6" s="4">
-        <v>0.125</v>
+        <f>B6</f>
+        <v>7.1499999999999994E-2</v>
       </c>
       <c r="D6" s="34">
-        <v>0.22900000000000001</v>
+        <v>7.1199999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26497,6 +26453,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="C7" s="4">
+        <f>B7</f>
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="D7" s="34">

</xml_diff>